<commit_message>
Update portfolio-updates.xlsx on 2025-08-18 13:08:11
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,6 +471,22 @@
         <v>318.3999938964844</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-08-18</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>58.06999969482422</v>
+      </c>
+      <c r="C3" t="n">
+        <v>676</v>
+      </c>
+      <c r="D3" t="n">
+        <v>314.8999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-19 13:02:21
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,6 +487,22 @@
         <v>314.8999938964844</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-08-19</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>59.59000015258789</v>
+      </c>
+      <c r="C4" t="n">
+        <v>700.25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>321.4500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-20 13:04:13
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,6 +503,22 @@
         <v>321.4500122070312</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-08-20</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>59.84999847412109</v>
+      </c>
+      <c r="C5" t="n">
+        <v>689.5999755859375</v>
+      </c>
+      <c r="D5" t="n">
+        <v>326.5499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-21 13:03:04
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,22 @@
         <v>326.5499877929688</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-08-21</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>58.15999984741211</v>
+      </c>
+      <c r="C6" t="n">
+        <v>685.4000244140625</v>
+      </c>
+      <c r="D6" t="n">
+        <v>321.7999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-22 13:01:55
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +535,22 @@
         <v>321.7999877929688</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>58.5099983215332</v>
+      </c>
+      <c r="C7" t="n">
+        <v>680.2999877929688</v>
+      </c>
+      <c r="D7" t="n">
+        <v>319.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-23 12:57:51
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,6 +551,22 @@
         <v>319.1000061035156</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-08-23</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>58.5099983215332</v>
+      </c>
+      <c r="C8" t="n">
+        <v>680.2999877929688</v>
+      </c>
+      <c r="D8" t="n">
+        <v>319.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-24 12:58:29
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,6 +567,22 @@
         <v>319.1000061035156</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-08-24</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>58.5099983215332</v>
+      </c>
+      <c r="C9" t="n">
+        <v>680.2999877929688</v>
+      </c>
+      <c r="D9" t="n">
+        <v>319.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-25 13:04:30
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,6 +583,22 @@
         <v>319.1000061035156</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-08-25</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>57.43000030517578</v>
+      </c>
+      <c r="C10" t="n">
+        <v>686.7999877929688</v>
+      </c>
+      <c r="D10" t="n">
+        <v>319.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-26 13:05:23
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -599,6 +599,22 @@
         <v>319.25</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-08-26</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>56.97000122070312</v>
+      </c>
+      <c r="C11" t="n">
+        <v>681.6500244140625</v>
+      </c>
+      <c r="D11" t="n">
+        <v>317.8999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-27 13:01:34
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,6 +615,22 @@
         <v>317.8999938964844</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-27</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>57.09999847412109</v>
+      </c>
+      <c r="C12" t="n">
+        <v>680.5499877929688</v>
+      </c>
+      <c r="D12" t="n">
+        <v>320.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-28 13:01:52
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,22 @@
         <v>320.75</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-08-28</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>56.31999969482422</v>
+      </c>
+      <c r="C13" t="n">
+        <v>675.4500122070312</v>
+      </c>
+      <c r="D13" t="n">
+        <v>315.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-29 13:00:11
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -647,6 +647,22 @@
         <v>315.5</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-08-29</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>56.43000030517578</v>
+      </c>
+      <c r="C14" t="n">
+        <v>669</v>
+      </c>
+      <c r="D14" t="n">
+        <v>313.9500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-30 12:55:28
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,6 +663,22 @@
         <v>313.9500122070312</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>56.43000030517578</v>
+      </c>
+      <c r="C15" t="n">
+        <v>669</v>
+      </c>
+      <c r="D15" t="n">
+        <v>313.9500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-08-31 12:56:38
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,6 +679,22 @@
         <v>313.9500122070312</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>56.43000030517578</v>
+      </c>
+      <c r="C16" t="n">
+        <v>669</v>
+      </c>
+      <c r="D16" t="n">
+        <v>313.9500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-01 13:02:55
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -695,6 +695,22 @@
         <v>313.9500122070312</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-09-01</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>57.86000061035156</v>
+      </c>
+      <c r="C17" t="n">
+        <v>690.1500244140625</v>
+      </c>
+      <c r="D17" t="n">
+        <v>321.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-02 13:02:50
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,6 +711,22 @@
         <v>321.1000061035156</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>58.25</v>
+      </c>
+      <c r="C18" t="n">
+        <v>684.4000244140625</v>
+      </c>
+      <c r="D18" t="n">
+        <v>322.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-03 13:00:24
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -727,6 +727,22 @@
         <v>322.3999938964844</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>57.9900016784668</v>
+      </c>
+      <c r="C19" t="n">
+        <v>692.0499877929688</v>
+      </c>
+      <c r="D19" t="n">
+        <v>326.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-04 12:58:27
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,6 +743,22 @@
         <v>326.1000061035156</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-09-04</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>57.41999816894531</v>
+      </c>
+      <c r="C20" t="n">
+        <v>687.5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>326.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-05 12:59:24
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,6 +759,22 @@
         <v>326.25</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-09-05</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>57.86999893188477</v>
+      </c>
+      <c r="C21" t="n">
+        <v>691.7000122070312</v>
+      </c>
+      <c r="D21" t="n">
+        <v>329.1499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-06 12:53:39
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -775,6 +775,22 @@
         <v>329.1499938964844</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>57.86999893188477</v>
+      </c>
+      <c r="C22" t="n">
+        <v>691.7000122070312</v>
+      </c>
+      <c r="D22" t="n">
+        <v>329.1499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-07 12:54:36
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -791,6 +791,22 @@
         <v>329.1499938964844</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>57.86999893188477</v>
+      </c>
+      <c r="C23" t="n">
+        <v>691.7000122070312</v>
+      </c>
+      <c r="D23" t="n">
+        <v>329.1499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-08 13:03:32
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,6 +807,22 @@
         <v>329.1499938964844</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>57.45000076293945</v>
+      </c>
+      <c r="C24" t="n">
+        <v>719.5</v>
+      </c>
+      <c r="D24" t="n">
+        <v>329.6499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-09 13:04:11
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,6 +823,22 @@
         <v>329.6499938964844</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>57.06000137329102</v>
+      </c>
+      <c r="C25" t="n">
+        <v>715.5499877929688</v>
+      </c>
+      <c r="D25" t="n">
+        <v>325.7000122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-10 13:00:09
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,6 +839,22 @@
         <v>325.7000122070312</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>57.56999969482422</v>
+      </c>
+      <c r="C26" t="n">
+        <v>709.0999755859375</v>
+      </c>
+      <c r="D26" t="n">
+        <v>324.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-11 12:59:22
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,22 @@
         <v>324.3999938964844</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>56.93999862670898</v>
+      </c>
+      <c r="C27" t="n">
+        <v>705.8499755859375</v>
+      </c>
+      <c r="D27" t="n">
+        <v>328.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-12 12:58:06
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,6 +871,22 @@
         <v>328.1000061035156</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>57.11000061035156</v>
+      </c>
+      <c r="C28" t="n">
+        <v>715.25</v>
+      </c>
+      <c r="D28" t="n">
+        <v>321.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-13 12:53:56
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -887,6 +887,22 @@
         <v>321.3999938964844</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-09-13</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>57.11000061035156</v>
+      </c>
+      <c r="C29" t="n">
+        <v>715.25</v>
+      </c>
+      <c r="D29" t="n">
+        <v>321.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-14 12:53:41
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,6 +903,22 @@
         <v>321.3999938964844</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-09-14</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>57.11000061035156</v>
+      </c>
+      <c r="C30" t="n">
+        <v>715.25</v>
+      </c>
+      <c r="D30" t="n">
+        <v>321.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-15 13:01:49
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -919,6 +919,22 @@
         <v>321.3999938964844</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-09-15</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>58.06999969482422</v>
+      </c>
+      <c r="C31" t="n">
+        <v>712.9000244140625</v>
+      </c>
+      <c r="D31" t="n">
+        <v>323.2999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-16 13:01:23
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -935,6 +935,22 @@
         <v>323.2999877929688</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>58.97999954223633</v>
+      </c>
+      <c r="C32" t="n">
+        <v>713.25</v>
+      </c>
+      <c r="D32" t="n">
+        <v>327.2999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-17 13:01:29
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -951,6 +951,22 @@
         <v>327.2999877929688</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-09-17</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>59.29000091552734</v>
+      </c>
+      <c r="C33" t="n">
+        <v>719.1500244140625</v>
+      </c>
+      <c r="D33" t="n">
+        <v>328.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-18 13:00:52
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -967,6 +967,22 @@
         <v>328.25</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-09-18</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>59.08000183105469</v>
+      </c>
+      <c r="C34" t="n">
+        <v>711.2000122070312</v>
+      </c>
+      <c r="D34" t="n">
+        <v>337.8500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-19 13:00:22
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -983,6 +983,22 @@
         <v>337.8500061035156</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>60.40000152587891</v>
+      </c>
+      <c r="C35" t="n">
+        <v>707.4500122070312</v>
+      </c>
+      <c r="D35" t="n">
+        <v>336.5499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-20 12:56:21
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -999,6 +999,22 @@
         <v>336.5499877929688</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-09-20</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>60.40000152587891</v>
+      </c>
+      <c r="C36" t="n">
+        <v>707.4500122070312</v>
+      </c>
+      <c r="D36" t="n">
+        <v>336.5499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-21 12:55:25
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1015,6 +1015,22 @@
         <v>336.5499877929688</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-09-21</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>60.40000152587891</v>
+      </c>
+      <c r="C37" t="n">
+        <v>707.4500122070312</v>
+      </c>
+      <c r="D37" t="n">
+        <v>336.5499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-22 13:02:50
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1031,6 +1031,22 @@
         <v>336.5499877929688</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-09-22</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>59.93000030517578</v>
+      </c>
+      <c r="C38" t="n">
+        <v>696.25</v>
+      </c>
+      <c r="D38" t="n">
+        <v>341.8500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-23 13:01:02
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1047,6 +1047,22 @@
         <v>341.8500061035156</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-09-23</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>58.75</v>
+      </c>
+      <c r="C39" t="n">
+        <v>701.3499755859375</v>
+      </c>
+      <c r="D39" t="n">
+        <v>338.3500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-24 13:01:39
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1063,6 +1063,22 @@
         <v>338.3500061035156</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-09-24</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>57.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>682.9500122070312</v>
+      </c>
+      <c r="D40" t="n">
+        <v>335.7999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-25 13:02:35
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1079,6 +1079,22 @@
         <v>335.7999877929688</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-09-25</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>56.63999938964844</v>
+      </c>
+      <c r="C41" t="n">
+        <v>664.2999877929688</v>
+      </c>
+      <c r="D41" t="n">
+        <v>332.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-26 13:01:00
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1095,6 +1095,22 @@
         <v>332.25</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-09-26</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>55.27999877929688</v>
+      </c>
+      <c r="C42" t="n">
+        <v>672.9000244140625</v>
+      </c>
+      <c r="D42" t="n">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-27 12:54:46
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1111,6 +1111,22 @@
         <v>321</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-09-27</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>55.27999877929688</v>
+      </c>
+      <c r="C43" t="n">
+        <v>672.9000244140625</v>
+      </c>
+      <c r="D43" t="n">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-28 12:55:37
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1127,6 +1127,22 @@
         <v>321</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-09-28</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>55.27999877929688</v>
+      </c>
+      <c r="C44" t="n">
+        <v>672.9000244140625</v>
+      </c>
+      <c r="D44" t="n">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-29 13:03:38
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1143,6 +1143,22 @@
         <v>321</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-09-29</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>55.27999877929688</v>
+      </c>
+      <c r="C45" t="n">
+        <v>672.5</v>
+      </c>
+      <c r="D45" t="n">
+        <v>324.8500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-09-30 13:03:32
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,6 +1159,22 @@
         <v>324.8500061035156</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-09-30</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>55.04999923706055</v>
+      </c>
+      <c r="C46" t="n">
+        <v>680.2000122070312</v>
+      </c>
+      <c r="D46" t="n">
+        <v>325.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-01 13:03:38
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1175,6 +1175,22 @@
         <v>325.5</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>55.18000030517578</v>
+      </c>
+      <c r="C47" t="n">
+        <v>718.3499755859375</v>
+      </c>
+      <c r="D47" t="n">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-02 12:59:17
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1191,6 +1191,22 @@
         <v>329</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>55.20000076293945</v>
+      </c>
+      <c r="C48" t="n">
+        <v>718</v>
+      </c>
+      <c r="D48" t="n">
+        <v>329.4500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-03 12:58:56
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1207,6 +1207,22 @@
         <v>329.4500122070312</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>54.45999908447266</v>
+      </c>
+      <c r="C49" t="n">
+        <v>716.0999755859375</v>
+      </c>
+      <c r="D49" t="n">
+        <v>328.4500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-04 12:54:59
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1223,6 +1223,22 @@
         <v>328.4500122070312</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>54.45999908447266</v>
+      </c>
+      <c r="C50" t="n">
+        <v>716.0999755859375</v>
+      </c>
+      <c r="D50" t="n">
+        <v>328.4500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-05 12:55:23
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,6 +1239,22 @@
         <v>328.4500122070312</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-10-05</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>54.45999908447266</v>
+      </c>
+      <c r="C51" t="n">
+        <v>716.0999755859375</v>
+      </c>
+      <c r="D51" t="n">
+        <v>328.4500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-06 13:02:29
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1255,6 +1255,22 @@
         <v>328.4500122070312</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>54.11000061035156</v>
+      </c>
+      <c r="C52" t="n">
+        <v>712.6500244140625</v>
+      </c>
+      <c r="D52" t="n">
+        <v>335.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-07 13:02:30
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1271,6 +1271,22 @@
         <v>335.1000061035156</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>54.0099983215332</v>
+      </c>
+      <c r="C53" t="n">
+        <v>698.0499877929688</v>
+      </c>
+      <c r="D53" t="n">
+        <v>337.8500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-08 13:02:43
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1287,6 +1287,22 @@
         <v>337.8500061035156</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-10-08</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>52.77000045776367</v>
+      </c>
+      <c r="C54" t="n">
+        <v>681.5499877929688</v>
+      </c>
+      <c r="D54" t="n">
+        <v>341.6499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-09 13:03:10
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1303,6 +1303,22 @@
         <v>341.6499938964844</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-10-09</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>53.16999816894531</v>
+      </c>
+      <c r="C55" t="n">
+        <v>681.0999755859375</v>
+      </c>
+      <c r="D55" t="n">
+        <v>345.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-10 13:00:43
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1319,6 +1319,22 @@
         <v>345.5</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>54.31000137329102</v>
+      </c>
+      <c r="C56" t="n">
+        <v>678.9500122070312</v>
+      </c>
+      <c r="D56" t="n">
+        <v>348.2999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-11 12:55:09
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,6 +1335,22 @@
         <v>348.2999877929688</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-10-11</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>54.31000137329102</v>
+      </c>
+      <c r="C57" t="n">
+        <v>678.9500122070312</v>
+      </c>
+      <c r="D57" t="n">
+        <v>348.2999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-12 12:55:23
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1351,6 +1351,22 @@
         <v>348.2999877929688</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-10-12</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>54.31000137329102</v>
+      </c>
+      <c r="C58" t="n">
+        <v>678.9500122070312</v>
+      </c>
+      <c r="D58" t="n">
+        <v>348.2999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-13 13:03:31
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1367,6 +1367,22 @@
         <v>348.2999877929688</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-10-13</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>54.34999847412109</v>
+      </c>
+      <c r="C59" t="n">
+        <v>660.75</v>
+      </c>
+      <c r="D59" t="n">
+        <v>348.3500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-14 13:04:23
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1383,6 +1383,22 @@
         <v>348.3500061035156</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-10-14</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>53.95000076293945</v>
+      </c>
+      <c r="C60" t="n">
+        <v>395.4500122070312</v>
+      </c>
+      <c r="D60" t="n">
+        <v>347.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-15 13:04:26
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1399,6 +1399,22 @@
         <v>347.75</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-10-15</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>53.72999954223633</v>
+      </c>
+      <c r="C61" t="n">
+        <v>390.8500061035156</v>
+      </c>
+      <c r="D61" t="n">
+        <v>354.3500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-16 13:04:28
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1415,6 +1415,22 @@
         <v>354.3500061035156</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-10-16</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>53.61000061035156</v>
+      </c>
+      <c r="C62" t="n">
+        <v>396.7999877929688</v>
+      </c>
+      <c r="D62" t="n">
+        <v>347.8500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-17 13:02:05
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1431,6 +1431,22 @@
         <v>347.8500061035156</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-10-17</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>52.91999816894531</v>
+      </c>
+      <c r="C63" t="n">
+        <v>396.6000061035156</v>
+      </c>
+      <c r="D63" t="n">
+        <v>342.6499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-18 12:56:27
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1447,6 +1447,22 @@
         <v>342.6499938964844</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-10-18</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>52.91999816894531</v>
+      </c>
+      <c r="C64" t="n">
+        <v>396.6000061035156</v>
+      </c>
+      <c r="D64" t="n">
+        <v>342.6499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-19 12:56:11
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1463,6 +1463,22 @@
         <v>342.6499938964844</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-10-19</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>52.91999816894531</v>
+      </c>
+      <c r="C65" t="n">
+        <v>396.6000061035156</v>
+      </c>
+      <c r="D65" t="n">
+        <v>342.6499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-20 13:03:13
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1479,6 +1479,22 @@
         <v>342.6499938964844</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-10-20</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>53.09000015258789</v>
+      </c>
+      <c r="C66" t="n">
+        <v>399.75</v>
+      </c>
+      <c r="D66" t="n">
+        <v>338.1499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-21 13:05:50
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1495,6 +1495,22 @@
         <v>338.1499938964844</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-10-21</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>54.18000030517578</v>
+      </c>
+      <c r="C67" t="n">
+        <v>401.8500061035156</v>
+      </c>
+      <c r="D67" t="n">
+        <v>338.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-22 13:06:19
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1511,6 +1511,22 @@
         <v>338.1000061035156</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>54.18000030517578</v>
+      </c>
+      <c r="C68" t="n">
+        <v>401.8500061035156</v>
+      </c>
+      <c r="D68" t="n">
+        <v>338.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-23 13:05:12
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1527,6 +1527,22 @@
         <v>338.1000061035156</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-10-23</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>54.52999877929688</v>
+      </c>
+      <c r="C69" t="n">
+        <v>405.8500061035156</v>
+      </c>
+      <c r="D69" t="n">
+        <v>328.3500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-24 13:04:13
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1543,6 +1543,22 @@
         <v>328.3500061035156</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-10-24</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>53.81999969482422</v>
+      </c>
+      <c r="C70" t="n">
+        <v>405.7999877929688</v>
+      </c>
+      <c r="D70" t="n">
+        <v>326.6000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-25 12:56:14
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1559,6 +1559,22 @@
         <v>326.6000061035156</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>53.81999969482422</v>
+      </c>
+      <c r="C71" t="n">
+        <v>403.2999877929688</v>
+      </c>
+      <c r="D71" t="n">
+        <v>326.6000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-26 12:57:42
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1575,6 +1575,22 @@
         <v>326.6000061035156</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-10-26</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>53.81999969482422</v>
+      </c>
+      <c r="C72" t="n">
+        <v>403.2999877929688</v>
+      </c>
+      <c r="D72" t="n">
+        <v>326.6000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-27 13:04:59
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1591,6 +1591,19 @@
         <v>326.6000061035156</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>53.70999908447266</v>
+      </c>
+      <c r="C73" t="n">
+        <v>333.7000122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-28 13:03:54
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1604,6 +1604,19 @@
         <v>333.7000122070312</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-10-28</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>56.22000122070312</v>
+      </c>
+      <c r="C74" t="n">
+        <v>334.6000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-29 13:06:05
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1617,6 +1617,19 @@
         <v>334.6000061035156</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>58.18999862670898</v>
+      </c>
+      <c r="C75" t="n">
+        <v>330.4500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-30 13:04:52
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1630,6 +1630,19 @@
         <v>330.4500122070312</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-10-30</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>58.5099983215332</v>
+      </c>
+      <c r="C76" t="n">
+        <v>329.3500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-10-31 13:03:31
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1643,6 +1643,19 @@
         <v>329.3500061035156</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>59.29999923706055</v>
+      </c>
+      <c r="C77" t="n">
+        <v>317.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-01 12:56:53
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1656,6 +1656,22 @@
         <v>317.75</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>59.29999923706055</v>
+      </c>
+      <c r="C78" t="n">
+        <v>410</v>
+      </c>
+      <c r="D78" t="n">
+        <v>317.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-02 12:56:13
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1672,6 +1672,22 @@
         <v>317.75</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>59.29999923706055</v>
+      </c>
+      <c r="C79" t="n">
+        <v>410</v>
+      </c>
+      <c r="D79" t="n">
+        <v>317.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-03 13:04:34
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1688,6 +1688,19 @@
         <v>317.75</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-11-03</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>59.2400016784668</v>
+      </c>
+      <c r="C80" t="n">
+        <v>322.6000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-04 13:07:42
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1701,6 +1701,19 @@
         <v>322.6000061035156</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>59.9900016784668</v>
+      </c>
+      <c r="C81" t="n">
+        <v>313.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-05 13:05:18
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1714,6 +1714,19 @@
         <v>313.5</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-11-05</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>60.04999923706055</v>
+      </c>
+      <c r="C82" t="n">
+        <v>313.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-06 13:04:38
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1727,6 +1727,19 @@
         <v>313.5</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>59.61000061035156</v>
+      </c>
+      <c r="C83" t="n">
+        <v>305.6499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-07 13:02:36
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1740,6 +1740,19 @@
         <v>305.6499938964844</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>57.38000106811523</v>
+      </c>
+      <c r="C84" t="n">
+        <v>306.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-08 12:57:15
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1753,6 +1753,22 @@
         <v>306.1000061035156</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-11-08</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>57.38000106811523</v>
+      </c>
+      <c r="C85" t="n">
+        <v>405.7000122070312</v>
+      </c>
+      <c r="D85" t="n">
+        <v>306.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-09 12:57:15
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1769,6 +1769,22 @@
         <v>306.1000061035156</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-11-09</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>57.38000106811523</v>
+      </c>
+      <c r="C86" t="n">
+        <v>405.7000122070312</v>
+      </c>
+      <c r="D86" t="n">
+        <v>306.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-10 13:05:38
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1785,6 +1785,19 @@
         <v>306.1000061035156</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-11-10</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>57.43000030517578</v>
+      </c>
+      <c r="C87" t="n">
+        <v>301.4500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-11 13:05:18
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D87"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1798,6 +1798,19 @@
         <v>301.4500122070312</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-11-11</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>57.81999969482422</v>
+      </c>
+      <c r="C88" t="n">
+        <v>305.7999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-12 13:06:36
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1811,6 +1811,19 @@
         <v>305.7999877929688</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>58.47999954223633</v>
+      </c>
+      <c r="C89" t="n">
+        <v>308.7999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-13 13:06:21
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1824,6 +1824,19 @@
         <v>308.7999877929688</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>57.58000183105469</v>
+      </c>
+      <c r="C90" t="n">
+        <v>297.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-14 13:03:31
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1837,6 +1837,19 @@
         <v>297.75</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-11-14</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>57.68000030517578</v>
+      </c>
+      <c r="C91" t="n">
+        <v>303.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-15 12:58:08
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1850,6 +1850,22 @@
         <v>303.75</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-11-15</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>57.68000030517578</v>
+      </c>
+      <c r="C92" t="n">
+        <v>391.2000122070312</v>
+      </c>
+      <c r="D92" t="n">
+        <v>303.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-16 12:57:32
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1866,6 +1866,22 @@
         <v>303.75</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-11-16</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>57.68000030517578</v>
+      </c>
+      <c r="C93" t="n">
+        <v>391.2000122070312</v>
+      </c>
+      <c r="D93" t="n">
+        <v>303.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-17 13:05:29
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1882,6 +1882,19 @@
         <v>303.75</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-11-17</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>57.70000076293945</v>
+      </c>
+      <c r="C94" t="n">
+        <v>309.5499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-18 13:05:10
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1895,6 +1895,19 @@
         <v>309.5499877929688</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-11-18</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>56.90000152587891</v>
+      </c>
+      <c r="C95" t="n">
+        <v>306.1499938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-19 13:05:28
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1908,6 +1908,19 @@
         <v>306.1499938964844</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-11-19</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>56.52999877929688</v>
+      </c>
+      <c r="C96" t="n">
+        <v>306.6000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-20 13:04:04
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1921,6 +1921,19 @@
         <v>306.6000061035156</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-11-20</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>56.70000076293945</v>
+      </c>
+      <c r="C97" t="n">
+        <v>306.8999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-21 13:02:44
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1934,6 +1934,19 @@
         <v>306.8999938964844</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-11-21</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>55.09999847412109</v>
+      </c>
+      <c r="C98" t="n">
+        <v>301.9500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-22 12:56:54
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1947,6 +1947,22 @@
         <v>301.9500122070312</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-11-22</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>55.09999847412109</v>
+      </c>
+      <c r="C99" t="n">
+        <v>362.25</v>
+      </c>
+      <c r="D99" t="n">
+        <v>301.9500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-23 12:56:22
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1963,6 +1963,22 @@
         <v>301.9500122070312</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-11-23</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>55.09999847412109</v>
+      </c>
+      <c r="C100" t="n">
+        <v>362.25</v>
+      </c>
+      <c r="D100" t="n">
+        <v>301.9500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-24 13:06:13
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1979,6 +1979,19 @@
         <v>301.9500122070312</v>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-11-24</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>54.61000061035156</v>
+      </c>
+      <c r="C101" t="n">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-25 13:06:16
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1992,6 +1992,19 @@
         <v>301</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-11-25</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>54.18999862670898</v>
+      </c>
+      <c r="C102" t="n">
+        <v>302.2999877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-26 13:07:56
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2005,6 +2005,19 @@
         <v>302.2999877929688</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-11-26</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>55.58000183105469</v>
+      </c>
+      <c r="C103" t="n">
+        <v>306.8500061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-27 13:05:55
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2018,6 +2018,19 @@
         <v>306.8500061035156</v>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-11-27</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>54.93000030517578</v>
+      </c>
+      <c r="C104" t="n">
+        <v>302.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-28 13:04:00
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2031,6 +2031,19 @@
         <v>302.75</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-11-28</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>54.0099983215332</v>
+      </c>
+      <c r="C105" t="n">
+        <v>300.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-29 13:00:20
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2044,6 +2044,22 @@
         <v>300.1000061035156</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-11-29</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>54.0099983215332</v>
+      </c>
+      <c r="C106" t="n">
+        <v>356.7999877929688</v>
+      </c>
+      <c r="D106" t="n">
+        <v>300.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-11-30 12:59:47
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2060,6 +2060,22 @@
         <v>300.1000061035156</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-11-30</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>54.0099983215332</v>
+      </c>
+      <c r="C107" t="n">
+        <v>356.7999877929688</v>
+      </c>
+      <c r="D107" t="n">
+        <v>300.1000061035156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-01 13:08:34
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2076,6 +2076,19 @@
         <v>300.1000061035156</v>
       </c>
     </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-12-01</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>53.72000122070312</v>
+      </c>
+      <c r="C108" t="n">
+        <v>301.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-02 13:08:13
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2089,6 +2089,19 @@
         <v>301.5</v>
       </c>
     </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>53.41999816894531</v>
+      </c>
+      <c r="C109" t="n">
+        <v>300.5499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-03 13:08:39
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2102,6 +2102,19 @@
         <v>300.5499877929688</v>
       </c>
     </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-12-03</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>52.59000015258789</v>
+      </c>
+      <c r="C110" t="n">
+        <v>297.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-04 13:09:11
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2115,6 +2115,19 @@
         <v>297.75</v>
       </c>
     </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-12-04</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>50.84999847412109</v>
+      </c>
+      <c r="C111" t="n">
+        <v>295.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-05 13:05:35
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2128,6 +2128,19 @@
         <v>295.75</v>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>51.7400016784668</v>
+      </c>
+      <c r="C112" t="n">
+        <v>292.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-06 13:00:33
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2141,6 +2141,22 @@
         <v>292.3999938964844</v>
       </c>
     </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-12-06</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>51.7400016784668</v>
+      </c>
+      <c r="C113" t="n">
+        <v>353.6000061035156</v>
+      </c>
+      <c r="D113" t="n">
+        <v>292.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-07 12:59:03
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2157,6 +2157,22 @@
         <v>292.3999938964844</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-12-07</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>51.7400016784668</v>
+      </c>
+      <c r="C114" t="n">
+        <v>353.6000061035156</v>
+      </c>
+      <c r="D114" t="n">
+        <v>292.3999938964844</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-08 13:08:01
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2173,6 +2173,19 @@
         <v>292.3999938964844</v>
       </c>
     </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-12-08</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>51.77999877929688</v>
+      </c>
+      <c r="C115" t="n">
+        <v>285.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-09 13:09:08
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2186,6 +2186,19 @@
         <v>285.25</v>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-12-09</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>52.54999923706055</v>
+      </c>
+      <c r="C116" t="n">
+        <v>291.7000122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-10 13:09:23
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2199,6 +2199,19 @@
         <v>291.7000122070312</v>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-12-10</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>51.54000091552734</v>
+      </c>
+      <c r="C117" t="n">
+        <v>283.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-11 13:10:36
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D117"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2212,6 +2212,19 @@
         <v>283.25</v>
       </c>
     </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-12-11</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>52.04000091552734</v>
+      </c>
+      <c r="C118" t="n">
+        <v>290.9500122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-12 13:07:40
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2225,6 +2225,19 @@
         <v>290.9500122070312</v>
       </c>
     </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-12-12</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>53.02000045776367</v>
+      </c>
+      <c r="C119" t="n">
+        <v>298.0499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update portfolio-updates.xlsx on 2025-12-13 13:01:23
</commit_message>
<xml_diff>
--- a/portfolio-updates.xlsx
+++ b/portfolio-updates.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2238,6 +2238,22 @@
         <v>298.0499877929688</v>
       </c>
     </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-12-13</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>53.02000045776367</v>
+      </c>
+      <c r="C120" t="n">
+        <v>347.4500122070312</v>
+      </c>
+      <c r="D120" t="n">
+        <v>298.0499877929688</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>